<commit_message>
added error handling for resultviewer
</commit_message>
<xml_diff>
--- a/documentation/Implementation plan.xlsx
+++ b/documentation/Implementation plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhan.dang/Coder_Academy/terminal_app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhan.dang/Coder_Academy/terminal_app/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7969BCE-BA55-CA4E-81E3-F3346ABDE278}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D320F9-1E19-5A4B-9694-C03EA74CBD84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{2238E1B7-16D8-3B45-B312-80DE606DF43A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Development Plan</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Install TTY-Prompt gem</t>
-  </si>
-  <si>
-    <t>Methods/Classes</t>
   </si>
   <si>
     <t>Method: calculator</t>
@@ -109,9 +106,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>allow modify result only if have time</t>
-  </si>
-  <si>
     <t>option 1 - call calculator method</t>
   </si>
   <si>
@@ -125,13 +119,82 @@
   </si>
   <si>
     <t>grab patient name &amp; score from previous entries &amp; use to create instance object if possible</t>
+  </si>
+  <si>
+    <t>not implemented</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>patient class created but feature not implemented</t>
+  </si>
+  <si>
+    <t>deviated from initial plan</t>
+  </si>
+  <si>
+    <t>allow modify result only if have time. 
+Drug selector is just a drug list
+view result only
+patient med record not implemented but add med function added</t>
+  </si>
+  <si>
+    <t>add medication</t>
+  </si>
+  <si>
+    <t>on-the-fly notes</t>
+  </si>
+  <si>
+    <t>ARGV</t>
+  </si>
+  <si>
+    <t>Use ARGV to enable adding a med outside of the program itself</t>
+  </si>
+  <si>
+    <t>unable to make ARGV work with a class method. Have used a regular class method to enable adding medication for a patient</t>
+  </si>
+  <si>
+    <t>Use ARGV to add on-the-fly notes which will display face up to the user</t>
+  </si>
+  <si>
+    <t>displayed in table format</t>
+  </si>
+  <si>
+    <t>Error handling</t>
+  </si>
+  <si>
+    <t>Invalid selection from main menu</t>
+  </si>
+  <si>
+    <t>Handled in else statement to tell user that selection is invalid</t>
+  </si>
+  <si>
+    <t>CSV check for calculator method</t>
+  </si>
+  <si>
+    <t>Check that file exists. If it doesn't, warn user that results will not be saved and ask if want to continue</t>
+  </si>
+  <si>
+    <t>CSV check for view results method</t>
+  </si>
+  <si>
+    <t>Warn user that history doesn't exist and go back to main menu</t>
+  </si>
+  <si>
+    <t>Invalid name for view results</t>
+  </si>
+  <si>
+    <t>warn user that name doesn't exist in record</t>
+  </si>
+  <si>
+    <t>Methods/Classes/error types</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,13 +210,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -168,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -178,6 +254,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,31 +572,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A074F6-BF76-5840-925E-2CEB31FE4CCF}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -528,7 +622,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -536,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -561,7 +655,7 @@
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -572,7 +666,7 @@
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -583,10 +677,10 @@
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -597,7 +691,7 @@
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -608,63 +702,171 @@
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>43712</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
+      <c r="D13" t="s">
+        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>29</v>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>43712</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="6">
+        <v>43713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2">
+        <v>43713</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
manual testing spreadsheet completed
</commit_message>
<xml_diff>
--- a/documentation/Implementation plan.xlsx
+++ b/documentation/Implementation plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhan.dang/Coder_Academy/terminal_app/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D320F9-1E19-5A4B-9694-C03EA74CBD84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9CEF56-89F7-504A-818D-24526E97DBEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{2238E1B7-16D8-3B45-B312-80DE606DF43A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Development Plan</t>
   </si>
@@ -118,9 +118,6 @@
     <t>option 4 - call med record method</t>
   </si>
   <si>
-    <t>grab patient name &amp; score from previous entries &amp; use to create instance object if possible</t>
-  </si>
-  <si>
     <t>not implemented</t>
   </si>
   <si>
@@ -188,6 +185,12 @@
   </si>
   <si>
     <t>Methods/Classes/error types</t>
+  </si>
+  <si>
+    <t>if csv does not exist, rescue error message will display after user types in a name</t>
+  </si>
+  <si>
+    <t>grab patient name &amp; score from previous entries &amp; use to create instance object of a patient class if possible</t>
   </si>
 </sst>
 </file>
@@ -254,10 +257,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A074F6-BF76-5840-925E-2CEB31FE4CCF}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,29 +591,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -705,7 +708,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -733,10 +736,10 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -747,58 +750,76 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2">
+        <v>43712</v>
+      </c>
       <c r="F17" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -807,18 +828,18 @@
         <v>43712</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -829,32 +850,41 @@
     </row>
     <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="5">
+        <v>43713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="C22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="2">
         <v>43713</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
+      <c r="F22" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>

</xml_diff>